<commit_message>
Implementing multiple files support
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,51 +609,6 @@
           <t>Totale imponibile/importo</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Totale imposta</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>Riferimento normativo</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>Condizioni di pagamento</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Modalità</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Importo</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>Istituto finanziario</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Codice IBAN</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Nome dell'allegato</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Formato</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -834,49 +789,544 @@
           <t xml:space="preserve"> 1400.00</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT01879020517</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FPR12</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0000000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> monservicesrls@pec.it</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FSNMRC74C14F109F</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fattura a saldo per lavori edili svolti c/o vs cantiere sito in Carpignano</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RF01 (ordinario)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LE</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 73040</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TD01 (fattura)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> EUR</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT04879980755</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 04879980755</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1.00</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NR</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0.00</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> inv.cont. - subappalto nel settore edile</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
         <is>
           <t xml:space="preserve"> TP02 (pagamento completo)</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
+      <c r="AG3" t="inlineStr">
         <is>
           <t xml:space="preserve"> MP05 (bonifico)</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1400.00</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Banca Popolare Pugliese</t>
-        </is>
-      </c>
-      <c r="AQ2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IT09A0526279700CC0590060768</t>
-        </is>
-      </c>
-      <c r="AR2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Fattura 9-2022 - 18-03-2022.pdf</t>
-        </is>
-      </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> pdf</t>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2022-04-11 (11 Aprile 2022)</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> INTESA SAN PAOLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT01879020517</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FPR12</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0000000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> monservicesrls@pec.it</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FSNMRC74C14F109F</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fattura a saldo per lavori edili di ristrutturazione effettuati per vs conto c/o</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RF01 (ordinario)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LE</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 73040</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TD01 (fattura)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> EUR</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT04879980755</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 04879980755</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1.00</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NR</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TP02 (pagamento completo)</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MP05 (bonifico)</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2022-04-11 (11 Aprile 2022)</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> INTESA SAN PAOLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT01879020517</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FPR12</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0000000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> monservicesrls@pec.it</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FSNMRC74C14F109F</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fattura di cappotto, rasato, smontaggio e montaggio marmi c/o immobile</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RF01 (ordinario)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LE</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 73040</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TD01 (fattura)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> EUR</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT04879980755</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 04879980755</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1.00</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NR</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TP02 (pagamento completo)</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MP05 (bonifico)</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2022-04-29 (29 Aprile 2022)</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> INTESA SAN PAOLO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved managing different fields over files
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AY5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +609,81 @@
           <t>Totale imponibile/importo</t>
         </is>
       </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Totale imposta</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Riferimento normativo</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Condizioni di pagamento</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Modalità</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Importo</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Istituto finanziario</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Codice IBAN</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Nome dell'allegato</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Formato</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>E-mail</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Codice Fiscale</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Descrizione bene/servizio</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Quantità</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Unità di misura</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Data scadenza pagamento</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -789,6 +864,57 @@
           <t xml:space="preserve"> 1400.00</t>
         </is>
       </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> inv.cont. - subappalto nel settore edile</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TP02 (pagamento completo)</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MP05 (bonifico)</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1400.00</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Banca Popolare Pugliese</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT09A0526279700CC0590060768</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fattura 9-2022 - 18-03-2022.pdf</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> pdf</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -821,152 +947,179 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t xml:space="preserve"> IT04879980755</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FSNMRC74C14F109F</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RF01 (ordinario)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 73045</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LEVERANO</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LE</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TD01 (fattura)</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> EUR</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 1</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> FSNMRC74C14F109F</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TP02 (pagamento completo)</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MP05 (bonifico)</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2500.00</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> INTESA SAN PAOLO</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT61Z0306980094100000002981</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> donatogiaffreda@libero.it</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 04879980755</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Fattura a saldo per lavori edili svolti c/o vs cantiere sito in Carpignano</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> RF01 (ordinario)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> LE</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 73040</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IT</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TD01 (fattura)</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> EUR</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2500.00</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IT04879980755</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 04879980755</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
+      <c r="AW3" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1.00</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="AX3" t="inlineStr">
         <is>
           <t xml:space="preserve"> NR</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2500.00</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2500.00</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2500.00</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TP02 (pagamento completo)</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> MP05 (bonifico)</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
+      <c r="AY3" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2022-04-11 (11 Aprile 2022)</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2500.00</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> INTESA SAN PAOLO</t>
         </is>
       </c>
     </row>
@@ -1001,152 +1154,179 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t xml:space="preserve"> IT04879980755</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FSNMRC74C14F109F</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RF01 (ordinario)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 73045</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LEVERANO</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LE</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TD01 (fattura)</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> EUR</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 1</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> FSNMRC74C14F109F</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TP02 (pagamento completo)</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MP05 (bonifico)</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000.00</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> INTESA SAN PAOLO</t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT61Z0306980094100000002981</t>
+        </is>
+      </c>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> donatogiaffreda@libero.it</t>
+        </is>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 04879980755</t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Fattura a saldo per lavori edili di ristrutturazione effettuati per vs conto c/o</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> RF01 (ordinario)</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> LE</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 73040</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IT</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TD01 (fattura)</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> EUR</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 6000.00</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IT04879980755</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 04879980755</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
+      <c r="AW4" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1.00</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="AX4" t="inlineStr">
         <is>
           <t xml:space="preserve"> NR</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 6000.00</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 6000.00</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 6000.00</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TP02 (pagamento completo)</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> MP05 (bonifico)</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
+      <c r="AY4" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2022-04-11 (11 Aprile 2022)</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 6000.00</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> INTESA SAN PAOLO</t>
         </is>
       </c>
     </row>
@@ -1181,152 +1361,179 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t xml:space="preserve"> IT04879980755</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FSNMRC74C14F109F</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RF01 (ordinario)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 73045</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LEVERANO</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LE</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TD01 (fattura)</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> EUR</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 1</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> FSNMRC74C14F109F</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.00</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
+        </is>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TP02 (pagamento completo)</t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MP05 (bonifico)</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8100.00</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> INTESA SAN PAOLO</t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IT61Z0306980094100000002981</t>
+        </is>
+      </c>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> donatogiaffreda@libero.it</t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 04879980755</t>
+        </is>
+      </c>
+      <c r="AV5" t="inlineStr">
         <is>
           <t xml:space="preserve"> Fattura di cappotto, rasato, smontaggio e montaggio marmi c/o immobile</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> RF01 (ordinario)</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> LE</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 73040</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IT</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TD01 (fattura)</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> EUR</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8100.00</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IT04879980755</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 04879980755</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> MON SERVICE SOCIETA' A RESPONSABILITA' LIMITATA SEMPLIFICATA</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TENUTA SPECCHIA, 2</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
+      <c r="AW5" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1.00</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="AX5" t="inlineStr">
         <is>
           <t xml:space="preserve"> NR</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8100.00</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8100.00</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N6.3 (inversione contabile - subappalto nel settore edile)</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8100.00</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.00</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Reverse charge subappalto nel settore edile Art. 17, c. 6 lett. a), DPR 633/72</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TP02 (pagamento completo)</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> MP05 (bonifico)</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
+      <c r="AY5" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2022-04-29 (29 Aprile 2022)</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8100.00</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> INTESA SAN PAOLO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added user control and developed script
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>